<commit_message>
FRE: lists (user, products, orders)
</commit_message>
<xml_diff>
--- a/_Adminstratives/Frontend/Abgabe 1/01_Listenansichten.xlsx
+++ b/_Adminstratives/Frontend/Abgabe 1/01_Listenansichten.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\_Daten\5_Fortbildung\517 Junior SWE (2025)\Projekt\In-crust-we-trust\_Adminstratives\Frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\_Daten\5_Fortbildung\517 Junior SWE (2025)\Projekt\In-crust-we-trust\_Adminstratives\Frontend\Abgabe 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4AA56D-B4ED-4383-AB36-221755C47563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B5A6F3-9D2E-42B3-B43D-FFC8BD51D472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E10166A8-70FE-43CE-9965-9295F8FFC1A0}"/>
   </bookViews>
@@ -575,20 +575,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4851,7 +4851,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4970,18 +4970,18 @@
       <c r="J6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="19">
         <v>4020</v>
       </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="16">
+      <c r="L6" s="19"/>
+      <c r="M6" s="18">
         <v>45352</v>
       </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16">
+      <c r="N6" s="18"/>
+      <c r="O6" s="18">
         <v>45669</v>
       </c>
-      <c r="P6" s="16"/>
+      <c r="P6" s="18"/>
       <c r="Q6" s="3" t="s">
         <v>46</v>
       </c>
@@ -5008,14 +5008,14 @@
         <v>8010</v>
       </c>
       <c r="L7" s="17"/>
-      <c r="M7" s="15">
+      <c r="M7" s="16">
         <v>45394</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15">
+      <c r="N7" s="16"/>
+      <c r="O7" s="16">
         <v>45734</v>
       </c>
-      <c r="P7" s="15"/>
+      <c r="P7" s="16"/>
       <c r="Q7" t="s">
         <v>70</v>
       </c>
@@ -5044,14 +5044,14 @@
         <v>5020</v>
       </c>
       <c r="L8" s="17"/>
-      <c r="M8" s="15">
+      <c r="M8" s="16">
         <v>45450</v>
       </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15">
+      <c r="N8" s="16"/>
+      <c r="O8" s="16">
         <v>45618</v>
       </c>
-      <c r="P8" s="15"/>
+      <c r="P8" s="16"/>
       <c r="Q8" s="4" t="s">
         <v>46</v>
       </c>
@@ -5082,14 +5082,14 @@
         <v>2700</v>
       </c>
       <c r="L9" s="17"/>
-      <c r="M9" s="15">
+      <c r="M9" s="16">
         <v>45492</v>
       </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15">
+      <c r="N9" s="16"/>
+      <c r="O9" s="16">
         <v>45568</v>
       </c>
-      <c r="P9" s="15"/>
+      <c r="P9" s="16"/>
       <c r="Q9" s="4" t="s">
         <v>46</v>
       </c>
@@ -5120,14 +5120,14 @@
         <v>6850</v>
       </c>
       <c r="L10" s="17"/>
-      <c r="M10" s="15">
+      <c r="M10" s="16">
         <v>45527</v>
       </c>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15">
+      <c r="N10" s="16"/>
+      <c r="O10" s="16">
         <v>45661</v>
       </c>
-      <c r="P10" s="15"/>
+      <c r="P10" s="16"/>
       <c r="Q10" s="4" t="s">
         <v>46</v>
       </c>
@@ -5158,14 +5158,14 @@
         <v>4400</v>
       </c>
       <c r="L11" s="17"/>
-      <c r="M11" s="15">
+      <c r="M11" s="16">
         <v>45565</v>
       </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15">
+      <c r="N11" s="16"/>
+      <c r="O11" s="16">
         <v>45749</v>
       </c>
-      <c r="P11" s="15"/>
+      <c r="P11" s="16"/>
       <c r="Q11" s="4" t="s">
         <v>46</v>
       </c>
@@ -5196,14 +5196,14 @@
         <v>9500</v>
       </c>
       <c r="L12" s="17"/>
-      <c r="M12" s="15">
+      <c r="M12" s="16">
         <v>45606</v>
       </c>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15">
+      <c r="N12" s="16"/>
+      <c r="O12" s="16">
         <v>45703</v>
       </c>
-      <c r="P12" s="15"/>
+      <c r="P12" s="16"/>
       <c r="Q12" t="s">
         <v>70</v>
       </c>
@@ -5234,14 +5234,14 @@
         <v>3430</v>
       </c>
       <c r="L13" s="17"/>
-      <c r="M13" s="15">
+      <c r="M13" s="16">
         <v>45662</v>
       </c>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15">
+      <c r="N13" s="16"/>
+      <c r="O13" s="16">
         <v>45743</v>
       </c>
-      <c r="P13" s="15"/>
+      <c r="P13" s="16"/>
       <c r="Q13" s="4" t="s">
         <v>46</v>
       </c>
@@ -5272,14 +5272,14 @@
         <v>3100</v>
       </c>
       <c r="L14" s="17"/>
-      <c r="M14" s="15">
+      <c r="M14" s="16">
         <v>45679</v>
       </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15">
+      <c r="N14" s="16"/>
+      <c r="O14" s="16">
         <v>45787</v>
       </c>
-      <c r="P14" s="15"/>
+      <c r="P14" s="16"/>
       <c r="Q14" s="4" t="s">
         <v>46</v>
       </c>
@@ -5310,14 +5310,14 @@
         <v>7000</v>
       </c>
       <c r="L15" s="17"/>
-      <c r="M15" s="15">
+      <c r="M15" s="16">
         <v>45702</v>
       </c>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15">
+      <c r="N15" s="16"/>
+      <c r="O15" s="16">
         <v>45776</v>
       </c>
-      <c r="P15" s="15"/>
+      <c r="P15" s="16"/>
       <c r="Q15" s="4" t="s">
         <v>46</v>
       </c>
@@ -5348,14 +5348,14 @@
         <v>1190</v>
       </c>
       <c r="L16" s="17"/>
-      <c r="M16" s="15">
+      <c r="M16" s="16">
         <v>45717</v>
       </c>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15">
+      <c r="N16" s="16"/>
+      <c r="O16" s="16">
         <v>45778</v>
       </c>
-      <c r="P16" s="15"/>
+      <c r="P16" s="16"/>
       <c r="Q16" s="4" t="s">
         <v>46</v>
       </c>
@@ -5386,14 +5386,14 @@
         <v>9560</v>
       </c>
       <c r="L17" s="17"/>
-      <c r="M17" s="15">
+      <c r="M17" s="16">
         <v>45744</v>
       </c>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15">
+      <c r="N17" s="16"/>
+      <c r="O17" s="16">
         <v>45790</v>
       </c>
-      <c r="P17" s="15"/>
+      <c r="P17" s="16"/>
       <c r="Q17" s="4" t="s">
         <v>46</v>
       </c>
@@ -5424,14 +5424,14 @@
         <v>2500</v>
       </c>
       <c r="L18" s="17"/>
-      <c r="M18" s="15">
+      <c r="M18" s="16">
         <v>45757</v>
       </c>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15">
+      <c r="N18" s="16"/>
+      <c r="O18" s="16">
         <v>45793</v>
       </c>
-      <c r="P18" s="15"/>
+      <c r="P18" s="16"/>
       <c r="Q18" s="4" t="s">
         <v>46</v>
       </c>
@@ -5443,13 +5443,22 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="K17:L17"/>
@@ -5466,22 +5475,13 @@
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -5496,8 +5496,8 @@
   </sheetPr>
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5597,14 +5597,14 @@
         <v>5.9</v>
       </c>
       <c r="J6" s="12"/>
-      <c r="K6" s="16">
+      <c r="K6" s="18">
         <v>45352</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16">
+      <c r="L6" s="18"/>
+      <c r="M6" s="18">
         <v>45669</v>
       </c>
-      <c r="N6" s="16"/>
+      <c r="N6" s="18"/>
       <c r="O6" s="3" t="s">
         <v>46</v>
       </c>
@@ -5625,14 +5625,14 @@
         <v>7.2</v>
       </c>
       <c r="J7" s="13"/>
-      <c r="K7" s="15">
+      <c r="K7" s="16">
         <v>45394</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15">
+      <c r="L7" s="16"/>
+      <c r="M7" s="16">
         <v>45734</v>
       </c>
-      <c r="N7" s="15"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="4" t="s">
         <v>70</v>
       </c>
@@ -5653,14 +5653,14 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="J8" s="13"/>
-      <c r="K8" s="15">
+      <c r="K8" s="16">
         <v>45450</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15">
+      <c r="L8" s="16"/>
+      <c r="M8" s="16">
         <v>45618</v>
       </c>
-      <c r="N8" s="15"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="4" t="s">
         <v>70</v>
       </c>
@@ -5681,14 +5681,14 @@
         <v>3.5</v>
       </c>
       <c r="J9" s="13"/>
-      <c r="K9" s="15">
+      <c r="K9" s="16">
         <v>45492</v>
       </c>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15">
+      <c r="L9" s="16"/>
+      <c r="M9" s="16">
         <v>45568</v>
       </c>
-      <c r="N9" s="15"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="4" t="s">
         <v>46</v>
       </c>
@@ -5709,14 +5709,14 @@
         <v>11.5</v>
       </c>
       <c r="J10" s="13"/>
-      <c r="K10" s="15">
+      <c r="K10" s="16">
         <v>45527</v>
       </c>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15">
+      <c r="L10" s="16"/>
+      <c r="M10" s="16">
         <v>45661</v>
       </c>
-      <c r="N10" s="15"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="4" t="s">
         <v>46</v>
       </c>
@@ -5737,14 +5737,14 @@
         <v>8.9</v>
       </c>
       <c r="J11" s="13"/>
-      <c r="K11" s="15">
+      <c r="K11" s="16">
         <v>45565</v>
       </c>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15">
+      <c r="L11" s="16"/>
+      <c r="M11" s="16">
         <v>45749</v>
       </c>
-      <c r="N11" s="15"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="4" t="s">
         <v>46</v>
       </c>
@@ -5765,14 +5765,14 @@
         <v>5.4</v>
       </c>
       <c r="J12" s="13"/>
-      <c r="K12" s="15">
+      <c r="K12" s="16">
         <v>45606</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15">
+      <c r="L12" s="16"/>
+      <c r="M12" s="16">
         <v>45703</v>
       </c>
-      <c r="N12" s="15"/>
+      <c r="N12" s="16"/>
       <c r="O12" s="4" t="s">
         <v>46</v>
       </c>
@@ -5793,14 +5793,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="J13" s="13"/>
-      <c r="K13" s="15">
+      <c r="K13" s="16">
         <v>45662</v>
       </c>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15">
+      <c r="L13" s="16"/>
+      <c r="M13" s="16">
         <v>45743</v>
       </c>
-      <c r="N13" s="15"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="4" t="s">
         <v>46</v>
       </c>
@@ -5823,14 +5823,14 @@
         <v>8.9</v>
       </c>
       <c r="J14" s="13"/>
-      <c r="K14" s="15">
+      <c r="K14" s="16">
         <v>45679</v>
       </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15">
+      <c r="L14" s="16"/>
+      <c r="M14" s="16">
         <v>45787</v>
       </c>
-      <c r="N14" s="15"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="4" t="s">
         <v>46</v>
       </c>
@@ -5853,14 +5853,14 @@
         <v>10.5</v>
       </c>
       <c r="J15" s="13"/>
-      <c r="K15" s="15">
+      <c r="K15" s="16">
         <v>45702</v>
       </c>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15">
+      <c r="L15" s="16"/>
+      <c r="M15" s="16">
         <v>45776</v>
       </c>
-      <c r="N15" s="15"/>
+      <c r="N15" s="16"/>
       <c r="O15" s="4" t="s">
         <v>46</v>
       </c>
@@ -5883,14 +5883,14 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="J16" s="13"/>
-      <c r="K16" s="15">
+      <c r="K16" s="16">
         <v>45717</v>
       </c>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15">
+      <c r="L16" s="16"/>
+      <c r="M16" s="16">
         <v>45778</v>
       </c>
-      <c r="N16" s="15"/>
+      <c r="N16" s="16"/>
       <c r="O16" s="4" t="s">
         <v>70</v>
       </c>
@@ -5913,14 +5913,14 @@
         <v>11.2</v>
       </c>
       <c r="J17" s="13"/>
-      <c r="K17" s="15">
+      <c r="K17" s="16">
         <v>45744</v>
       </c>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15">
+      <c r="L17" s="16"/>
+      <c r="M17" s="16">
         <v>45790</v>
       </c>
-      <c r="N17" s="15"/>
+      <c r="N17" s="16"/>
       <c r="O17" s="4" t="s">
         <v>46</v>
       </c>
@@ -5943,14 +5943,14 @@
         <v>11.5</v>
       </c>
       <c r="J18" s="13"/>
-      <c r="K18" s="15">
+      <c r="K18" s="16">
         <v>45702</v>
       </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15">
+      <c r="L18" s="16"/>
+      <c r="M18" s="16">
         <v>45776</v>
       </c>
-      <c r="N18" s="15"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="4" t="s">
         <v>46</v>
       </c>
@@ -5973,14 +5973,14 @@
         <v>10.9</v>
       </c>
       <c r="J19" s="13"/>
-      <c r="K19" s="15">
+      <c r="K19" s="16">
         <v>45717</v>
       </c>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15">
+      <c r="L19" s="16"/>
+      <c r="M19" s="16">
         <v>45778</v>
       </c>
-      <c r="N19" s="15"/>
+      <c r="N19" s="16"/>
       <c r="O19" s="4" t="s">
         <v>46</v>
       </c>
@@ -6003,14 +6003,14 @@
         <v>11</v>
       </c>
       <c r="J20" s="13"/>
-      <c r="K20" s="15">
+      <c r="K20" s="16">
         <v>45744</v>
       </c>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15">
+      <c r="L20" s="16"/>
+      <c r="M20" s="16">
         <v>45790</v>
       </c>
-      <c r="N20" s="15"/>
+      <c r="N20" s="16"/>
       <c r="O20" s="4" t="s">
         <v>46</v>
       </c>
@@ -6033,14 +6033,14 @@
         <v>10.199999999999999</v>
       </c>
       <c r="J21" s="13"/>
-      <c r="K21" s="15">
+      <c r="K21" s="16">
         <v>45702</v>
       </c>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15">
+      <c r="L21" s="16"/>
+      <c r="M21" s="16">
         <v>45776</v>
       </c>
-      <c r="N21" s="15"/>
+      <c r="N21" s="16"/>
       <c r="O21" s="4" t="s">
         <v>70</v>
       </c>
@@ -6063,14 +6063,14 @@
         <v>11.9</v>
       </c>
       <c r="J22" s="13"/>
-      <c r="K22" s="15">
+      <c r="K22" s="16">
         <v>45717</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15">
+      <c r="L22" s="16"/>
+      <c r="M22" s="16">
         <v>45778</v>
       </c>
-      <c r="N22" s="15"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="4" t="s">
         <v>46</v>
       </c>
@@ -6093,14 +6093,14 @@
         <v>10.5</v>
       </c>
       <c r="J23" s="13"/>
-      <c r="K23" s="15">
+      <c r="K23" s="16">
         <v>45744</v>
       </c>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15">
+      <c r="L23" s="16"/>
+      <c r="M23" s="16">
         <v>45790</v>
       </c>
-      <c r="N23" s="15"/>
+      <c r="N23" s="16"/>
       <c r="O23" s="4" t="s">
         <v>46</v>
       </c>
@@ -6123,14 +6123,14 @@
         <v>9.9</v>
       </c>
       <c r="J24" s="13"/>
-      <c r="K24" s="15">
+      <c r="K24" s="16">
         <v>45702</v>
       </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15">
+      <c r="L24" s="16"/>
+      <c r="M24" s="16">
         <v>45776</v>
       </c>
-      <c r="N24" s="15"/>
+      <c r="N24" s="16"/>
       <c r="O24" s="4" t="s">
         <v>70</v>
       </c>
@@ -6153,14 +6153,14 @@
         <v>13.2</v>
       </c>
       <c r="J25" s="13"/>
-      <c r="K25" s="15">
+      <c r="K25" s="16">
         <v>45717</v>
       </c>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15">
+      <c r="L25" s="16"/>
+      <c r="M25" s="16">
         <v>45778</v>
       </c>
-      <c r="N25" s="15"/>
+      <c r="N25" s="16"/>
       <c r="O25" s="4" t="s">
         <v>46</v>
       </c>
@@ -6181,14 +6181,14 @@
         <v>5.9</v>
       </c>
       <c r="J26" s="13"/>
-      <c r="K26" s="15">
+      <c r="K26" s="16">
         <v>45744</v>
       </c>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15">
+      <c r="L26" s="16"/>
+      <c r="M26" s="16">
         <v>45790</v>
       </c>
-      <c r="N26" s="15"/>
+      <c r="N26" s="16"/>
       <c r="O26" s="4" t="s">
         <v>46</v>
       </c>
@@ -6209,14 +6209,14 @@
         <v>5.8</v>
       </c>
       <c r="J27" s="13"/>
-      <c r="K27" s="15">
+      <c r="K27" s="16">
         <v>45702</v>
       </c>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15">
+      <c r="L27" s="16"/>
+      <c r="M27" s="16">
         <v>45776</v>
       </c>
-      <c r="N27" s="15"/>
+      <c r="N27" s="16"/>
       <c r="O27" s="4" t="s">
         <v>46</v>
       </c>
@@ -6237,14 +6237,14 @@
         <v>6.2</v>
       </c>
       <c r="J28" s="13"/>
-      <c r="K28" s="15">
+      <c r="K28" s="16">
         <v>45702</v>
       </c>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15">
+      <c r="L28" s="16"/>
+      <c r="M28" s="16">
         <v>45776</v>
       </c>
-      <c r="N28" s="15"/>
+      <c r="N28" s="16"/>
       <c r="O28" s="4" t="s">
         <v>46</v>
       </c>
@@ -6265,14 +6265,14 @@
         <v>4.5</v>
       </c>
       <c r="J29" s="13"/>
-      <c r="K29" s="15">
+      <c r="K29" s="16">
         <v>45717</v>
       </c>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15">
+      <c r="L29" s="16"/>
+      <c r="M29" s="16">
         <v>45778</v>
       </c>
-      <c r="N29" s="15"/>
+      <c r="N29" s="16"/>
       <c r="O29" s="4" t="s">
         <v>46</v>
       </c>
@@ -6293,14 +6293,14 @@
         <v>6.5</v>
       </c>
       <c r="J30" s="13"/>
-      <c r="K30" s="15">
+      <c r="K30" s="16">
         <v>45744</v>
       </c>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15">
+      <c r="L30" s="16"/>
+      <c r="M30" s="16">
         <v>45790</v>
       </c>
-      <c r="N30" s="15"/>
+      <c r="N30" s="16"/>
       <c r="O30" s="4" t="s">
         <v>46</v>
       </c>
@@ -6321,14 +6321,14 @@
         <v>7</v>
       </c>
       <c r="J31" s="13"/>
-      <c r="K31" s="15">
+      <c r="K31" s="16">
         <v>45702</v>
       </c>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15">
+      <c r="L31" s="16"/>
+      <c r="M31" s="16">
         <v>45776</v>
       </c>
-      <c r="N31" s="15"/>
+      <c r="N31" s="16"/>
       <c r="O31" s="4" t="s">
         <v>46</v>
       </c>
@@ -6351,14 +6351,14 @@
         <v>2.8</v>
       </c>
       <c r="J32" s="13"/>
-      <c r="K32" s="15">
+      <c r="K32" s="16">
         <v>45717</v>
       </c>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15">
+      <c r="L32" s="16"/>
+      <c r="M32" s="16">
         <v>45778</v>
       </c>
-      <c r="N32" s="15"/>
+      <c r="N32" s="16"/>
       <c r="O32" s="4" t="s">
         <v>46</v>
       </c>
@@ -6381,14 +6381,14 @@
         <v>2.5</v>
       </c>
       <c r="J33" s="13"/>
-      <c r="K33" s="15">
+      <c r="K33" s="16">
         <v>45744</v>
       </c>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15">
+      <c r="L33" s="16"/>
+      <c r="M33" s="16">
         <v>45790</v>
       </c>
-      <c r="N33" s="15"/>
+      <c r="N33" s="16"/>
       <c r="O33" s="4" t="s">
         <v>46</v>
       </c>
@@ -6411,14 +6411,14 @@
         <v>3.2</v>
       </c>
       <c r="J34" s="13"/>
-      <c r="K34" s="15">
+      <c r="K34" s="16">
         <v>45702</v>
       </c>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15">
+      <c r="L34" s="16"/>
+      <c r="M34" s="16">
         <v>45776</v>
       </c>
-      <c r="N34" s="15"/>
+      <c r="N34" s="16"/>
       <c r="O34" s="4" t="s">
         <v>46</v>
       </c>
@@ -6441,14 +6441,14 @@
         <v>4</v>
       </c>
       <c r="J35" s="13"/>
-      <c r="K35" s="15">
+      <c r="K35" s="16">
         <v>45717</v>
       </c>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15">
+      <c r="L35" s="16"/>
+      <c r="M35" s="16">
         <v>45778</v>
       </c>
-      <c r="N35" s="15"/>
+      <c r="N35" s="16"/>
       <c r="O35" s="4" t="s">
         <v>46</v>
       </c>
@@ -6471,14 +6471,14 @@
         <v>3.9</v>
       </c>
       <c r="J36" s="13"/>
-      <c r="K36" s="15">
+      <c r="K36" s="16">
         <v>45744</v>
       </c>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15">
+      <c r="L36" s="16"/>
+      <c r="M36" s="16">
         <v>45790</v>
       </c>
-      <c r="N36" s="15"/>
+      <c r="N36" s="16"/>
       <c r="O36" s="4" t="s">
         <v>46</v>
       </c>
@@ -6486,6 +6486,60 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:N32"/>
     <mergeCell ref="K36:L36"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="K33:L33"/>
@@ -6494,60 +6548,6 @@
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="K35:L35"/>
     <mergeCell ref="M35:N35"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:N32"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -6562,8 +6562,8 @@
   </sheetPr>
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6626,7 +6626,7 @@
       <c r="O3" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="P3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="Q3" s="6"/>
@@ -6674,10 +6674,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
-      <c r="D6" s="16">
+      <c r="D6" s="18">
         <v>45352</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="12">
         <v>116.4</v>
       </c>
@@ -6698,20 +6698,20 @@
       <c r="O6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="19">
         <v>4020</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="16">
+      <c r="Q6" s="19"/>
+      <c r="R6" s="18">
         <v>45352</v>
       </c>
-      <c r="S6" s="16"/>
+      <c r="S6" s="18"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="D7" s="15">
+      <c r="D7" s="16">
         <v>45394</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="13">
         <v>46.8</v>
       </c>
@@ -6732,17 +6732,17 @@
         <v>8010</v>
       </c>
       <c r="Q7" s="17"/>
-      <c r="R7" s="15">
+      <c r="R7" s="16">
         <v>45394</v>
       </c>
-      <c r="S7" s="15"/>
+      <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C8" s="4"/>
-      <c r="D8" s="15">
+      <c r="D8" s="16">
         <v>45450</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="13">
         <v>104.4</v>
       </c>
@@ -6767,17 +6767,17 @@
         <v>5020</v>
       </c>
       <c r="Q8" s="17"/>
-      <c r="R8" s="15">
+      <c r="R8" s="16">
         <v>45450</v>
       </c>
-      <c r="S8" s="15"/>
+      <c r="S8" s="16"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C9" s="4"/>
-      <c r="D9" s="15">
+      <c r="D9" s="16">
         <v>45492</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="13">
         <v>115.7</v>
       </c>
@@ -6802,17 +6802,17 @@
         <v>2700</v>
       </c>
       <c r="Q9" s="17"/>
-      <c r="R9" s="15">
+      <c r="R9" s="16">
         <v>45492</v>
       </c>
-      <c r="S9" s="15"/>
+      <c r="S9" s="16"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C10" s="4"/>
-      <c r="D10" s="15">
+      <c r="D10" s="16">
         <v>45527</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="13">
         <v>54.3</v>
       </c>
@@ -6833,17 +6833,17 @@
         <v>6850</v>
       </c>
       <c r="Q10" s="17"/>
-      <c r="R10" s="15">
+      <c r="R10" s="16">
         <v>45527</v>
       </c>
-      <c r="S10" s="15"/>
+      <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C11" s="4"/>
-      <c r="D11" s="15">
+      <c r="D11" s="16">
         <v>45565</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="13">
         <v>30.2</v>
       </c>
@@ -6868,17 +6868,17 @@
         <v>4400</v>
       </c>
       <c r="Q11" s="17"/>
-      <c r="R11" s="15">
+      <c r="R11" s="16">
         <v>45565</v>
       </c>
-      <c r="S11" s="15"/>
+      <c r="S11" s="16"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C12" s="4"/>
-      <c r="D12" s="15">
+      <c r="D12" s="16">
         <v>45606</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="13">
         <v>115</v>
       </c>
@@ -6903,17 +6903,17 @@
         <v>9500</v>
       </c>
       <c r="Q12" s="17"/>
-      <c r="R12" s="15">
+      <c r="R12" s="16">
         <v>45606</v>
       </c>
-      <c r="S12" s="15"/>
+      <c r="S12" s="16"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C13" s="4"/>
-      <c r="D13" s="15">
+      <c r="D13" s="16">
         <v>45662</v>
       </c>
-      <c r="E13" s="15"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="13">
         <v>68.900000000000006</v>
       </c>
@@ -6938,17 +6938,17 @@
         <v>3430</v>
       </c>
       <c r="Q13" s="17"/>
-      <c r="R13" s="15">
+      <c r="R13" s="16">
         <v>45662</v>
       </c>
-      <c r="S13" s="15"/>
+      <c r="S13" s="16"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C14" s="4"/>
-      <c r="D14" s="15">
+      <c r="D14" s="16">
         <v>45679</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="13">
         <v>34.700000000000003</v>
       </c>
@@ -6969,17 +6969,17 @@
         <v>3100</v>
       </c>
       <c r="Q14" s="17"/>
-      <c r="R14" s="15">
+      <c r="R14" s="16">
         <v>45679</v>
       </c>
-      <c r="S14" s="15"/>
+      <c r="S14" s="16"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C15" s="4"/>
-      <c r="D15" s="15">
+      <c r="D15" s="16">
         <v>45702</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="13">
         <v>133.9</v>
       </c>
@@ -7000,17 +7000,17 @@
         <v>7000</v>
       </c>
       <c r="Q15" s="17"/>
-      <c r="R15" s="15">
+      <c r="R15" s="16">
         <v>45702</v>
       </c>
-      <c r="S15" s="15"/>
+      <c r="S15" s="16"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C16" s="4"/>
-      <c r="D16" s="15">
+      <c r="D16" s="16">
         <v>45717</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="13">
         <v>82.4</v>
       </c>
@@ -7031,17 +7031,17 @@
         <v>1190</v>
       </c>
       <c r="Q16" s="17"/>
-      <c r="R16" s="15">
+      <c r="R16" s="16">
         <v>45717</v>
       </c>
-      <c r="S16" s="15"/>
+      <c r="S16" s="16"/>
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C17" s="4"/>
-      <c r="D17" s="15">
+      <c r="D17" s="16">
         <v>45744</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="13">
         <v>119.1</v>
       </c>
@@ -7066,17 +7066,17 @@
         <v>9560</v>
       </c>
       <c r="Q17" s="17"/>
-      <c r="R17" s="15">
+      <c r="R17" s="16">
         <v>45744</v>
       </c>
-      <c r="S17" s="15"/>
+      <c r="S17" s="16"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.35">
       <c r="C18" s="4"/>
-      <c r="D18" s="15">
+      <c r="D18" s="16">
         <v>45757</v>
       </c>
-      <c r="E18" s="15"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="13">
         <v>46.6</v>
       </c>
@@ -7101,18 +7101,31 @@
         <v>2500</v>
       </c>
       <c r="Q18" s="17"/>
-      <c r="R18" s="15">
+      <c r="R18" s="16">
         <v>45757</v>
       </c>
-      <c r="S18" s="15"/>
+      <c r="S18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="R13:S13"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="P18:Q18"/>
     <mergeCell ref="R18:S18"/>
@@ -7129,24 +7142,11 @@
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="R14:S14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>